<commit_message>
Updated readme + new spinners
</commit_message>
<xml_diff>
--- a/W-OP8/data/output/spreadsheets/Kodak_Lossless_True_Color_Image_Suite_tr0.1_max10_p1_g1_m0.05_x0.9_e2_t3_results.xlsx
+++ b/W-OP8/data/output/spreadsheets/Kodak_Lossless_True_Color_Image_Suite_tr0.1_max10_p1_g1_m0.05_x0.9_e2_t3_results.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Training" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Testing" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All Images" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -31,12 +32,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -57,11 +64,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +487,16 @@
           <t>baseline_mae</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>w8_0_5_13_10_8_4_6_fitness</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>w8_0_5_13_10_8_4_6_mae</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -495,9 +516,21 @@
       <c r="E2" t="n">
         <v>1179648</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>456214</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9.281697591145834</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-449952</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -517,9 +550,21 @@
       <c r="E3" t="n">
         <v>1179648</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>394400</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.024088541666666</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-386457</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -527,21 +572,26 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D4">
-        <f>SUM(D2:D3)</f>
-        <v/>
-      </c>
-      <c r="E4">
-        <f>SUM(E2:E3)</f>
-        <v/>
-      </c>
-      <c r="F4">
-        <f>SUM(F2:F3)</f>
-        <v/>
-      </c>
-      <c r="G4">
-        <f>AVERAGE(G2:G3)</f>
-        <v/>
+      <c r="D4" t="n">
+        <v>786432</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2359296</v>
+      </c>
+      <c r="F4" t="n">
+        <v>850614</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.65289306640625</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-836409</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -653,15 +703,33 @@
       <c r="E2" t="n">
         <v>1179648</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>500943</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10.19171142578125</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>497190</v>
+      </c>
+      <c r="J2" t="n">
+        <v>10.1153564453125</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>3753</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.07635498046875</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.7491870332552805</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -681,15 +749,33 @@
       <c r="E3" t="n">
         <v>1179648</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>478046</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9.725870768229166</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>465916</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9.479085286458334</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>12130</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.2467854817708321</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.537412717604582</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -709,15 +795,33 @@
       <c r="E4" t="n">
         <v>1179648</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>391854</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.9722900390625</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>383664</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7.8056640625</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>8190</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.1666259765625</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.090064156548102</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -737,15 +841,33 @@
       <c r="E5" t="n">
         <v>1179648</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>455834</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9.273966471354166</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>448468</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9.124104817708334</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>7366</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1498616536458321</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1.61593913573801</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -765,15 +887,33 @@
       <c r="E6" t="n">
         <v>1179648</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>427699</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8.701558430989584</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>421338</v>
+      </c>
+      <c r="J6" t="n">
+        <v>8.5721435546875</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6361</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.1294148763020839</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.487260900773675</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -793,15 +933,33 @@
       <c r="E7" t="n">
         <v>1179648</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>341927</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6.956522623697917</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>337485</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6.86614990234375</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4442</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.09037272135416696</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.299107704276059</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -821,15 +979,33 @@
       <c r="E8" t="n">
         <v>1179648</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>522907</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10.63857014973958</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>519862</v>
+      </c>
+      <c r="J8" t="n">
+        <v>10.57661946614583</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3045</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.06195068359374645</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.5823215218002437</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -849,15 +1025,33 @@
       <c r="E9" t="n">
         <v>1179648</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>456200</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9.281412760416666</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>448089</v>
+      </c>
+      <c r="J9" t="n">
+        <v>9.11639404296875</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>8111</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.1650187174479161</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.777948268303376</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -877,15 +1071,33 @@
       <c r="E10" t="n">
         <v>1179648</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>401282</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8.164103190104166</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>391618</v>
+      </c>
+      <c r="J10" t="n">
+        <v>7.967488606770833</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>9664</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.196614583333333</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2.408281457927343</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -905,15 +1117,33 @@
       <c r="E11" t="n">
         <v>1179648</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>483296</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9.832682291666666</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>477251</v>
+      </c>
+      <c r="J11" t="n">
+        <v>9.709696451822916</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>6045</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.12298583984375</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.250786267628948</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -933,15 +1163,33 @@
       <c r="E12" t="n">
         <v>1179648</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>433346</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.816446940104166</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>423271</v>
+      </c>
+      <c r="J12" t="n">
+        <v>8.611470540364584</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>10075</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.2049763997395821</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2.324932040448048</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -961,15 +1209,33 @@
       <c r="E13" t="n">
         <v>1179648</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>376433</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.658548990885417</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>367696</v>
+      </c>
+      <c r="J13" t="n">
+        <v>7.480794270833333</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>8737</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.1777547200520839</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2.32099736208037</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -989,15 +1255,33 @@
       <c r="E14" t="n">
         <v>1179648</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>408138</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.3035888671875</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>398650</v>
+      </c>
+      <c r="J14" t="n">
+        <v>8.110555013020834</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>9488</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.1930338541666661</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2.324703899171359</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1017,15 +1301,33 @@
       <c r="E15" t="n">
         <v>1179648</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>472926</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9.6217041015625</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>467173</v>
+      </c>
+      <c r="J15" t="n">
+        <v>9.504659016927084</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>5753</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.1170450846354161</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1.216469384216558</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1045,15 +1347,33 @@
       <c r="E16" t="n">
         <v>1179648</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>348655</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.093404134114583</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>341119</v>
+      </c>
+      <c r="J16" t="n">
+        <v>6.940083821614583</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>7536</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.1533203125</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2.16144899685936</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1073,15 +1393,33 @@
       <c r="E17" t="n">
         <v>1179648</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>404093</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8.221293131510416</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>397113</v>
+      </c>
+      <c r="J17" t="n">
+        <v>8.07928466796875</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>6980</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.1420084635416661</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.727325145449191</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1101,15 +1439,33 @@
       <c r="E18" t="n">
         <v>1179648</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>376638</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.6627197265625</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>369195</v>
+      </c>
+      <c r="J18" t="n">
+        <v>7.51129150390625</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>7443</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.15142822265625</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.976168097749032</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1129,15 +1485,33 @@
       <c r="E19" t="n">
         <v>1179648</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>560798</v>
+      </c>
+      <c r="G19" t="n">
+        <v>11.40946451822917</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>556699</v>
+      </c>
+      <c r="J19" t="n">
+        <v>11.32607014973958</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>4099</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.0833943684895857</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.7309227208370929</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1157,15 +1531,33 @@
       <c r="E20" t="n">
         <v>1179648</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>430179</v>
+      </c>
+      <c r="G20" t="n">
+        <v>8.75201416015625</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>423350</v>
+      </c>
+      <c r="J20" t="n">
+        <v>8.613077799479166</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>6829</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.1389363606770839</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1.587478700726907</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1185,15 +1577,33 @@
       <c r="E21" t="n">
         <v>1179648</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>524120</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10.66324869791667</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>513847</v>
+      </c>
+      <c r="J21" t="n">
+        <v>10.45424397786458</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>10273</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.2090047200520857</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1.960047317408227</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1213,15 +1623,33 @@
       <c r="E22" t="n">
         <v>1179648</v>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>399513</v>
+      </c>
+      <c r="G22" t="n">
+        <v>8.12811279296875</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>393486</v>
+      </c>
+      <c r="J22" t="n">
+        <v>8.0054931640625</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>6027</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.12261962890625</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1.508586704312501</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1241,15 +1669,33 @@
       <c r="E23" t="n">
         <v>1179648</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>440634</v>
+      </c>
+      <c r="G23" t="n">
+        <v>8.9647216796875</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>434855</v>
+      </c>
+      <c r="J23" t="n">
+        <v>8.847147623697916</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>5779</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.1175740559895839</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1.31151931081124</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1257,41 +1703,38 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D24">
-        <f>SUM(D2:D23)</f>
-        <v/>
-      </c>
-      <c r="E24">
-        <f>SUM(E2:E23)</f>
-        <v/>
-      </c>
-      <c r="F24">
-        <f>SUM(F2:F23)</f>
-        <v/>
-      </c>
-      <c r="G24">
-        <f>AVERAGE(G2:G23)</f>
-        <v/>
-      </c>
-      <c r="I24">
-        <f>SUM(I2:I23)</f>
-        <v/>
-      </c>
-      <c r="J24">
-        <f>AVERAGE(J2:J23)</f>
-        <v/>
-      </c>
-      <c r="L24">
-        <f>SUM(L2:L23)</f>
-        <v/>
-      </c>
-      <c r="M24">
-        <f>AVERAGE(M2:M23)</f>
-        <v/>
-      </c>
-      <c r="N24">
-        <f>AVERAGE(N2:N23)</f>
-        <v/>
+      <c r="D24" t="n">
+        <v>8650752</v>
+      </c>
+      <c r="E24" t="n">
+        <v>25952256</v>
+      </c>
+      <c r="F24" t="n">
+        <v>9635461</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8.910634358723957</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>9477335</v>
+      </c>
+      <c r="J24" t="n">
+        <v>8.764403372099906</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>158126</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.1462309866240529</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.679495856542068</v>
       </c>
     </row>
   </sheetData>
@@ -1403,15 +1846,33 @@
       <c r="E2" t="n">
         <v>1179648</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>456214</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9.281697591145834</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>449952</v>
+      </c>
+      <c r="J2" t="n">
+        <v>9.154296875</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>6262</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.1274007161458339</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.372601454580526</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1431,15 +1892,33 @@
       <c r="E3" t="n">
         <v>1179648</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>394400</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.024088541666666</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>386457</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7.86248779296875</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>7943</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.1616007486979161</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.01394523326572</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1459,15 +1938,33 @@
       <c r="E4" t="n">
         <v>1179648</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>500943</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10.19171142578125</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>497190</v>
+      </c>
+      <c r="J4" t="n">
+        <v>10.1153564453125</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3753</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.07635498046875</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.7491870332552805</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1487,15 +1984,33 @@
       <c r="E5" t="n">
         <v>1179648</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>478046</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9.725870768229166</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>465916</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9.479085286458334</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>12130</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.2467854817708321</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2.537412717604582</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1515,15 +2030,33 @@
       <c r="E6" t="n">
         <v>1179648</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>391854</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.9722900390625</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>383664</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7.8056640625</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>8190</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.1666259765625</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.090064156548102</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1543,15 +2076,33 @@
       <c r="E7" t="n">
         <v>1179648</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>455834</v>
+      </c>
+      <c r="G7" t="n">
+        <v>9.273966471354166</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>448468</v>
+      </c>
+      <c r="J7" t="n">
+        <v>9.124104817708334</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>7366</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.1498616536458321</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.61593913573801</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1571,15 +2122,33 @@
       <c r="E8" t="n">
         <v>1179648</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>427699</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.701558430989584</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>421338</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8.5721435546875</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>6361</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.1294148763020839</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.487260900773675</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1599,15 +2168,33 @@
       <c r="E9" t="n">
         <v>1179648</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>341927</v>
+      </c>
+      <c r="G9" t="n">
+        <v>6.956522623697917</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>337485</v>
+      </c>
+      <c r="J9" t="n">
+        <v>6.86614990234375</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4442</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.09037272135416696</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.299107704276059</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1627,15 +2214,33 @@
       <c r="E10" t="n">
         <v>1179648</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>522907</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10.63857014973958</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>519862</v>
+      </c>
+      <c r="J10" t="n">
+        <v>10.57661946614583</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3045</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.06195068359374645</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.5823215218002437</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1655,15 +2260,33 @@
       <c r="E11" t="n">
         <v>1179648</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>456200</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9.281412760416666</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>448089</v>
+      </c>
+      <c r="J11" t="n">
+        <v>9.11639404296875</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>8111</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.1650187174479161</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.777948268303376</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1683,15 +2306,33 @@
       <c r="E12" t="n">
         <v>1179648</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>401282</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.164103190104166</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>391618</v>
+      </c>
+      <c r="J12" t="n">
+        <v>7.967488606770833</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>9664</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.196614583333333</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2.408281457927343</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1711,15 +2352,33 @@
       <c r="E13" t="n">
         <v>1179648</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>483296</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9.832682291666666</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>477251</v>
+      </c>
+      <c r="J13" t="n">
+        <v>9.709696451822916</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>6045</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.12298583984375</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.250786267628948</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1739,15 +2398,33 @@
       <c r="E14" t="n">
         <v>1179648</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>433346</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.816446940104166</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>423271</v>
+      </c>
+      <c r="J14" t="n">
+        <v>8.611470540364584</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>10075</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.2049763997395821</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2.324932040448048</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1767,15 +2444,33 @@
       <c r="E15" t="n">
         <v>1179648</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>376433</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7.658548990885417</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>367696</v>
+      </c>
+      <c r="J15" t="n">
+        <v>7.480794270833333</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>8737</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.1777547200520839</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2.32099736208037</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1795,15 +2490,33 @@
       <c r="E16" t="n">
         <v>1179648</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>408138</v>
+      </c>
+      <c r="G16" t="n">
+        <v>8.3035888671875</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>398650</v>
+      </c>
+      <c r="J16" t="n">
+        <v>8.110555013020834</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>9488</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.1930338541666661</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2.324703899171359</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1823,15 +2536,33 @@
       <c r="E17" t="n">
         <v>1179648</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>472926</v>
+      </c>
+      <c r="G17" t="n">
+        <v>9.6217041015625</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>467173</v>
+      </c>
+      <c r="J17" t="n">
+        <v>9.504659016927084</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>5753</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.1170450846354161</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.216469384216558</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1851,15 +2582,33 @@
       <c r="E18" t="n">
         <v>1179648</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>348655</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.093404134114583</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>341119</v>
+      </c>
+      <c r="J18" t="n">
+        <v>6.940083821614583</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>7536</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.1533203125</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2.16144899685936</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1879,15 +2628,33 @@
       <c r="E19" t="n">
         <v>1179648</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>404093</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8.221293131510416</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>397113</v>
+      </c>
+      <c r="J19" t="n">
+        <v>8.07928466796875</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6980</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.1420084635416661</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1.727325145449191</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1907,15 +2674,33 @@
       <c r="E20" t="n">
         <v>1179648</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>376638</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.6627197265625</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>369195</v>
+      </c>
+      <c r="J20" t="n">
+        <v>7.51129150390625</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>7443</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.15142822265625</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1.976168097749032</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1935,15 +2720,33 @@
       <c r="E21" t="n">
         <v>1179648</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>560798</v>
+      </c>
+      <c r="G21" t="n">
+        <v>11.40946451822917</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>556699</v>
+      </c>
+      <c r="J21" t="n">
+        <v>11.32607014973958</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>4099</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.0833943684895857</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.7309227208370929</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1963,15 +2766,33 @@
       <c r="E22" t="n">
         <v>1179648</v>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>430179</v>
+      </c>
+      <c r="G22" t="n">
+        <v>8.75201416015625</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>423350</v>
+      </c>
+      <c r="J22" t="n">
+        <v>8.613077799479166</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>6829</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.1389363606770839</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1.587478700726907</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1991,15 +2812,33 @@
       <c r="E23" t="n">
         <v>1179648</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>524120</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10.66324869791667</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>513847</v>
+      </c>
+      <c r="J23" t="n">
+        <v>10.45424397786458</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>10273</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.2090047200520857</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1.960047317408227</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2019,15 +2858,33 @@
       <c r="E24" t="n">
         <v>1179648</v>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>399513</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8.12811279296875</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>393486</v>
+      </c>
+      <c r="J24" t="n">
+        <v>8.0054931640625</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>6027</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.12261962890625</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.508586704312501</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2047,15 +2904,33 @@
       <c r="E25" t="n">
         <v>1179648</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>440634</v>
+      </c>
+      <c r="G25" t="n">
+        <v>8.9647216796875</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>434855</v>
+      </c>
+      <c r="J25" t="n">
+        <v>8.847147623697916</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>5779</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.1175740559895839</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1.31151931081124</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2063,41 +2938,250 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D26">
-        <f>SUM(D2:D25)</f>
-        <v/>
-      </c>
-      <c r="E26">
-        <f>SUM(E2:E25)</f>
-        <v/>
-      </c>
-      <c r="F26">
-        <f>SUM(F2:F25)</f>
-        <v/>
-      </c>
-      <c r="G26">
-        <f>AVERAGE(G2:G25)</f>
-        <v/>
-      </c>
-      <c r="I26">
-        <f>SUM(I2:I25)</f>
-        <v/>
-      </c>
-      <c r="J26">
-        <f>AVERAGE(J2:J25)</f>
-        <v/>
-      </c>
-      <c r="L26">
-        <f>SUM(L2:L25)</f>
-        <v/>
-      </c>
-      <c r="M26">
-        <f>AVERAGE(M2:M25)</f>
-        <v/>
-      </c>
-      <c r="N26">
-        <f>AVERAGE(N2:N25)</f>
-        <v/>
+      <c r="D26" t="n">
+        <v>9437184</v>
+      </c>
+      <c r="E26" t="n">
+        <v>28311552</v>
+      </c>
+      <c r="F26" t="n">
+        <v>10486075</v>
+      </c>
+      <c r="G26" t="n">
+        <v>8.889155917697481</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>10313744</v>
+      </c>
+      <c r="J26" t="n">
+        <v>8.743069118923612</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>172331</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.1460867987738714</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1.68064398049049</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr"/>
+      <c r="B1" s="2" t="inlineStr"/>
+      <c r="C1" s="2" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Dataset Statistics:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Images Count</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>22</v>
+      </c>
+      <c r="C3" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Baseline Performance:</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Total Size (bytes)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>9,635,461</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10,486,075</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bits per Pixel</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8.911</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8.889</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>W-OP8 Performance:</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Total Size (bytes)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>9,477,335</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10,313,744</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Bits per Pixel</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>8.764</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>8.743</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Improvements:</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Size Reduction (bytes)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>158,126</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>172,331</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Size Reduction (%)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1.68%</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1.68%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bits per Pixel Improvement</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0.146</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.146</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>